<commit_message>
checks for min/max values, updates metadata accordingly, adds notes to clean_data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recaptures_metadata.xlsx
+++ b/data-raw/metadata/recaptures_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12D9A17-1216-4542-9659-F981CA683A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055E5CA7-4528-44E4-A40B-384934600E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1500" windowWidth="18390" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6730" yWindow="1440" windowWidth="15070" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>2007-01-02 09:15:00</t>
   </si>
   <si>
-    <t>2022-04-01 10:15:03</t>
-  </si>
-  <si>
     <t>Code for work that was done during visit to trap. Levels = c("Unplanned restart", "Continue trapping", "End trapping")</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   <si>
     <t>Life stage assigned based on visual observation and photo key of lifestages. Levels = c("Parr", "Button-up fry", "Silvery parr", "Not recorded", "Smolt", 
 "Fry")</t>
+  </si>
+  <si>
+    <t>202-04-01 10:45:43</t>
   </si>
 </sst>
 </file>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,7 +339,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="136" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -634,10 +633,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -751,7 +750,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -827,7 +826,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -864,8 +863,8 @@
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>64</v>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -903,7 +902,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1060,7 +1059,7 @@
         <v>53</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1081,7 +1080,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1195,7 +1194,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1233,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1271,7 +1270,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1309,7 +1308,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
completes tables metadata, writes clean csvs
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recaptures_metadata.xlsx
+++ b/data-raw/metadata/recaptures_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055E5CA7-4528-44E4-A40B-384934600E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E38BCD-1C51-47E9-AE2F-4CBAFF27CEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6730" yWindow="1440" windowWidth="15070" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2050" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -225,7 +225,10 @@
 "Fry")</t>
   </si>
   <si>
-    <t>202-04-01 10:45:43</t>
+    <t>2023-04-27 10:45:43</t>
+  </si>
+  <si>
+    <t>enumerated</t>
   </si>
 </sst>
 </file>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="136" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -645,7 +648,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -28866,7 +28869,7 @@
   <dimension ref="A1:Z927"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD34"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -28912,10 +28915,15 @@
       <c r="Z1" s="13"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="11">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>

</xml_diff>

<commit_message>
updates metadata recapture, release, checks release fish
</commit_message>
<xml_diff>
--- a/data-raw/metadata/recaptures_metadata.xlsx
+++ b/data-raw/metadata/recaptures_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12D9A17-1216-4542-9659-F981CA683A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E54C7C4-AF55-460A-A1F3-CFEF46786B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1500" windowWidth="18390" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3980" yWindow="1740" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>2007-01-02 09:15:00</t>
   </si>
   <si>
-    <t>2022-04-01 10:15:03</t>
-  </si>
-  <si>
     <t>Code for work that was done during visit to trap. Levels = c("Unplanned restart", "Continue trapping", "End trapping")</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   <si>
     <t>Life stage assigned based on visual observation and photo key of lifestages. Levels = c("Parr", "Button-up fry", "Silvery parr", "Not recorded", "Smolt", 
 "Fry")</t>
+  </si>
+  <si>
+    <t>2023-04-27 10:45:43</t>
   </si>
 </sst>
 </file>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,7 +339,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="136" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -634,10 +633,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -751,7 +750,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -827,7 +826,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -864,8 +863,8 @@
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>64</v>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -903,7 +902,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1060,7 +1059,7 @@
         <v>53</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1081,7 +1080,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1195,7 +1194,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1233,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1271,7 +1270,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1309,7 +1308,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>

</xml_diff>